<commit_message>
update results US capitals
</commit_message>
<xml_diff>
--- a/results_us.xlsx
+++ b/results_us.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\Uni\MASTER\3_Semester\physique_numerique_projet\projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F7A4B7-7875-4D74-8791-CC61D8B352B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC605AD1-A38E-45F9-A6A6-BADCFC6A23A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{D2F3FC73-D802-4D67-8216-6F6079696DC4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>T</t>
   </si>
@@ -85,13 +85,19 @@
   </si>
   <si>
     <t>best dD?</t>
+  </si>
+  <si>
+    <t>lowest d_final?</t>
+  </si>
+  <si>
+    <t>Plot the ones with lowest d_final</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,8 +105,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -126,13 +146,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -447,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810DE702-3022-4EED-9D62-710500BAAD47}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -458,42 +491,46 @@
     <col min="1" max="1" width="36.06640625" customWidth="1"/>
     <col min="6" max="6" width="21.46484375" customWidth="1"/>
     <col min="7" max="7" width="15.86328125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.59765625" customWidth="1"/>
+    <col min="9" max="9" width="13.59765625" customWidth="1"/>
+    <col min="11" max="11" width="17.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -517,7 +554,7 @@
         <v>-106167.1350381919</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C3">
         <v>2</v>
       </c>
@@ -531,11 +568,11 @@
         <v>2.2560000399999999E-2</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G36" si="0">E3-D3</f>
+        <f t="shared" ref="G3:G41" si="0">E3-D3</f>
         <v>-131718.82035035559</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C4">
         <v>3</v>
       </c>
@@ -555,26 +592,29 @@
       <c r="H4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C5">
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="4">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>150174.13707576299</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>46518.309973028299</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>2.2380000000000001E-2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="6">
         <f t="shared" si="0"/>
         <v>-103655.82710273469</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="C6">
         <v>5</v>
       </c>
@@ -591,548 +631,583 @@
         <f t="shared" si="0"/>
         <v>-99660.652997911588</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f>(G2+G3+G4+G5+G6)/5</f>
         <v>-114837.24156345046</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <f>(F2+F3+F4+F5+F6)/5</f>
         <v>2.2616000099999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>10000</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>161652.424740997</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>71234.970257119698</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.20490999500000001</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>-90417.4544838773</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C9">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>175520.92663185101</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>78778.888727637706</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>0.20802000200000001</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>-96742.037904213299</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C10">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C11">
         <v>3</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>157473.05340659199</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>66564.378873577996</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>0.205760002</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>-90908.674533013997</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C12">
         <v>4</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>169559.40028004901</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>79041.269369962494</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>0.20877000700000001</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>-90518.130910086518</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C12">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C13">
         <v>5</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>161514.09337264401</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>60752.035494780997</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>0.205039993</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>-100762.05787786302</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>9</v>
       </c>
-      <c r="I12">
-        <f>(G8+G9+G10+G11+G12)/5</f>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <f>(G9+G10+G11+G12+G13)/5</f>
         <v>-93869.671141810817</v>
       </c>
-      <c r="J12">
-        <f>(F8+F9+F10+F11+F12)/5</f>
+      <c r="K13">
+        <f>(F9+F10+F11+F12+F13)/5</f>
         <v>0.20649999980000003</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <v>100000</v>
       </c>
-      <c r="C14">
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D16">
         <v>165521.97055687799</v>
       </c>
-      <c r="E14">
+      <c r="E16">
         <v>35354.868621117799</v>
       </c>
-      <c r="F14">
+      <c r="F16">
         <v>0.101980001</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G16" s="2">
         <f t="shared" si="0"/>
         <v>-130167.10193576019</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C17">
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>173971.529243814</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>36494.7598894318</v>
       </c>
-      <c r="F15">
+      <c r="F17">
         <v>0.102519996</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G17" s="2">
         <f t="shared" si="0"/>
         <v>-137476.76935438221</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C16">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C18">
         <v>3</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <v>171652.62707595</v>
       </c>
-      <c r="E16">
+      <c r="E18">
         <v>37517.623964958402</v>
       </c>
-      <c r="F16">
+      <c r="F18">
         <v>0.100790001</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G18" s="2">
         <f t="shared" si="0"/>
         <v>-134135.00311099162</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C17">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C19">
         <v>4</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>170613.71035921801</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <v>36656.267581753003</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>0.104879998</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G19" s="2">
         <f t="shared" si="0"/>
         <v>-133957.44277746501</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C18">
+    <row r="20" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C20" s="4">
         <v>5</v>
       </c>
-      <c r="D18">
+      <c r="D20" s="4">
         <v>159739.233629222</v>
       </c>
-      <c r="E18">
+      <c r="E20" s="4">
         <v>34909.126163716901</v>
       </c>
-      <c r="F18">
+      <c r="F20" s="4">
         <v>0.100989997</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G20" s="6">
         <f t="shared" si="0"/>
         <v>-124830.10746550511</v>
       </c>
-      <c r="I18" s="3">
-        <f>(G14+G15+G16+G17+G18)/5</f>
+      <c r="I20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="3">
+        <f>(G16+G17+G18+G19+G20)/5</f>
         <v>-132113.28492882085</v>
       </c>
-      <c r="J18">
-        <f>(F14+F15+F16+F17+F18)/5</f>
+      <c r="K20" s="4">
+        <f>(F16+F17+F18+F19+F20)/5</f>
         <v>0.10223199860000001</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B20">
+      <c r="B23" s="4">
         <v>100000</v>
       </c>
-      <c r="C20">
+      <c r="C23" s="4">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D23" s="4">
         <v>159176.06146902699</v>
       </c>
-      <c r="E20">
+      <c r="E23" s="4">
         <v>36430.187453361097</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F23" s="5">
         <v>2.8260000100000002E-2</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G23" s="6">
         <f t="shared" si="0"/>
         <v>-122745.87401566589</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C21">
+      <c r="I23" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C24">
         <v>2</v>
       </c>
-      <c r="D21">
+      <c r="D24">
         <v>159443.108331358</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <v>50760.525101483901</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F24" s="1">
         <v>2.733E-2</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G24" s="2">
         <f t="shared" si="0"/>
         <v>-108682.5832298741</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C22">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C25">
         <v>3</v>
       </c>
-      <c r="D22">
+      <c r="D25">
         <v>161503.50369519001</v>
       </c>
-      <c r="E22">
+      <c r="E25">
         <v>45717.133201130797</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F25" s="1">
         <v>2.7009999400000002E-2</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G25" s="2">
         <f t="shared" si="0"/>
         <v>-115786.37049405921</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C23">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C26">
         <v>4</v>
       </c>
-      <c r="D23">
+      <c r="D26">
         <v>174330.73718925699</v>
       </c>
-      <c r="E23">
+      <c r="E26">
         <v>42248.556026284699</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F26" s="1">
         <v>2.8470000299999999E-2</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>-132082.18116297229</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C24">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C27">
         <v>5</v>
       </c>
-      <c r="D24">
+      <c r="D27">
         <v>148325.877026309</v>
       </c>
-      <c r="E24">
+      <c r="E27">
         <v>42718.225642254904</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F27" s="1">
         <v>2.8379999100000001E-2</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G27" s="2">
         <f t="shared" si="0"/>
         <v>-105607.6513840541</v>
       </c>
-      <c r="I24">
-        <f>(G20+G21+G22+G23+G24)/5</f>
+      <c r="J27">
+        <f>(G23+G24+G25+G26+G27)/5</f>
         <v>-116980.93205732512</v>
       </c>
-      <c r="J24" s="1">
-        <f>(F20+F21+F22+F23+F24)/5</f>
+      <c r="K27" s="1">
+        <f>(F23+F24+F25+F26+F27)/5</f>
         <v>2.7889999780000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>11</v>
       </c>
-      <c r="B26">
+      <c r="B30">
         <v>10000</v>
       </c>
-      <c r="C26">
+      <c r="C30">
         <v>1</v>
       </c>
-      <c r="D26">
+      <c r="D30">
         <v>167709.88696612601</v>
       </c>
-      <c r="E26">
+      <c r="E30">
         <v>40976.824184837802</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F30" s="1">
         <v>4.6110000499999998E-2</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G30" s="2">
         <f t="shared" si="0"/>
         <v>-126733.0627812882</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C27">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C31">
         <v>2</v>
       </c>
-      <c r="D27">
+      <c r="D31">
         <v>166225.91552140599</v>
       </c>
-      <c r="E27">
+      <c r="E31">
         <v>40780.8043399905</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F31" s="1">
         <v>4.7919999800000002E-2</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G31" s="2">
         <f t="shared" si="0"/>
         <v>-125445.11118141549</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C28">
+    <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C32" s="4">
         <v>3</v>
       </c>
-      <c r="D28">
+      <c r="D32" s="4">
         <v>149270.03754857299</v>
       </c>
-      <c r="E28">
+      <c r="E32" s="4">
         <v>38435.921554254302</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F32" s="5">
         <v>4.8749998199999998E-2</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G32" s="6">
         <f t="shared" si="0"/>
         <v>-110834.11599431868</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C29">
+      <c r="I32" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C33">
         <v>4</v>
       </c>
-      <c r="D29">
+      <c r="D33">
         <v>146813.01704760399</v>
       </c>
-      <c r="E29">
+      <c r="E33">
         <v>46441.087643156803</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F33" s="1">
         <v>4.6410001800000003E-2</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G33" s="2">
         <f t="shared" si="0"/>
         <v>-100371.92940444719</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="C30">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C34">
         <v>5</v>
       </c>
-      <c r="D30">
+      <c r="D34">
         <v>172952.41622676401</v>
       </c>
-      <c r="E30">
+      <c r="E34">
         <v>41808.689103532401</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F34" s="1">
         <v>4.8209998800000001E-2</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G34" s="2">
         <f t="shared" si="0"/>
         <v>-131143.7271232316</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H34" t="s">
         <v>9</v>
       </c>
-      <c r="I30">
-        <f>(G26+G27+G28+G29+G30)/5</f>
+      <c r="J34">
+        <f>(G30+G31+G32+G33+G34)/5</f>
         <v>-118905.58929694022</v>
       </c>
-      <c r="J30" s="1">
-        <f>(F26+F27+F28+F29+F30)/5</f>
+      <c r="K34" s="1">
+        <f>(F30+F31+F32+F33+F34)/5</f>
         <v>4.7479999819999993E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>13</v>
       </c>
-      <c r="B32">
+      <c r="B37">
         <v>100000</v>
       </c>
-      <c r="C32">
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D32">
+      <c r="D37">
         <v>166173.098665973</v>
       </c>
-      <c r="E32">
+      <c r="E37">
         <v>39688.300181258703</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F37" s="1">
         <v>4.7460001000000002E-2</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G37" s="2">
         <f t="shared" si="0"/>
         <v>-126484.79848471429</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.45">
-      <c r="C33">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C38">
         <v>2</v>
       </c>
-      <c r="D33">
+      <c r="D38">
         <v>144057.106573661</v>
       </c>
-      <c r="E33">
+      <c r="E38">
         <v>41395.9031583709</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F38" s="1">
         <v>5.1350001200000002E-2</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G38" s="2">
         <f t="shared" si="0"/>
         <v>-102661.2034152901</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.45">
-      <c r="C34">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C39">
         <v>3</v>
       </c>
-      <c r="D34">
+      <c r="D39">
         <v>139740.709855555</v>
       </c>
-      <c r="E34">
+      <c r="E39">
         <v>39410.650029363598</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F39" s="1">
         <v>4.8790000399999998E-2</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G39" s="2">
         <f t="shared" si="0"/>
         <v>-100330.0598261914</v>
       </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.45">
-      <c r="C35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C40">
         <v>4</v>
       </c>
-      <c r="D35">
+      <c r="D40">
         <v>148469.60189642399</v>
       </c>
-      <c r="E35">
+      <c r="E40">
         <v>39269.986569816501</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F40" s="1">
         <v>4.9320001199999998E-2</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G40" s="2">
         <f t="shared" si="0"/>
         <v>-109199.61532660748</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.45">
-      <c r="C36">
+    <row r="41" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C41" s="4">
         <v>5</v>
       </c>
-      <c r="D36">
+      <c r="D41" s="4">
         <v>188640.34425789301</v>
       </c>
-      <c r="E36">
+      <c r="E41" s="4">
         <v>38508.078196869399</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F41" s="5">
         <v>4.9240000499999999E-2</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G41" s="6">
         <f t="shared" si="0"/>
         <v>-150132.26606102361</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H41" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I36">
-        <f>(G32+G33+G34+G35+G36)/5</f>
+      <c r="I41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41" s="4">
+        <f>(G37+G38+G39+G40+G41)/5</f>
         <v>-117761.58862276538</v>
       </c>
-      <c r="J36" s="1">
-        <f>(F32+F33+F34+F35+F36)/5</f>
+      <c r="K41" s="5">
+        <f>(F37+F38+F39+F40+F41)/5</f>
         <v>4.923200086E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>